<commit_message>
sửa lỗi code train model 2 lần
</commit_message>
<xml_diff>
--- a/score_regression/Summit.xlsx
+++ b/score_regression/Summit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnMayHoc\score_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0839D8BF-0A40-4087-B0CC-A34C778608AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4032790-AC49-4D0E-8B50-1FF8B1E327D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB521FAA-9CC7-462A-8040-CEACDB6FA2CE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -458,7 +458,7 @@
   <dimension ref="A1:E663"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -544,7 +544,7 @@
         <v>271497</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -553,6 +553,15 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>271585</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-1216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Pred TH and CK
</commit_message>
<xml_diff>
--- a/score_regression/Summit.xlsx
+++ b/score_regression/Summit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnMayHoc\score_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A4911-F7B4-4D3F-AC9B-E2308273DD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC4D477-7410-4421-B34B-163B2B23E3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EB521FAA-9CC7-462A-8040-CEACDB6FA2CE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Scaling data</t>
+  </si>
+  <si>
+    <t>th_submit_1</t>
+  </si>
+  <si>
+    <t>ck_submit_1</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
   <dimension ref="A1:E663"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -597,10 +603,34 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
+      <c r="B8" s="2">
+        <v>271640</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2371</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>271644</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>